<commit_message>
ddl, dml e dql
</commit_message>
<xml_diff>
--- a/Op_flix/OPFLIX.xlsx
+++ b/Op_flix/OPFLIX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46938238804\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46938238804\Desktop\2s2019-sprint-1-bd\Op_flix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F9A058C-ED96-4BCB-AB17-76040A21F01A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA008E56-F3FE-445B-96AC-88B99F04EE57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{68A6FA9B-7148-4D9D-AD09-3F252A841521}"/>
   </bookViews>
@@ -279,40 +279,40 @@
     <t>400h</t>
   </si>
   <si>
-    <t>Breno</t>
-  </si>
-  <si>
-    <t>Gabriela</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
     <t>Débora</t>
   </si>
   <si>
-    <t>breno@gmail.com</t>
-  </si>
-  <si>
-    <t>gabriela@gmail.com</t>
-  </si>
-  <si>
-    <t>lucas@gmail.com</t>
-  </si>
-  <si>
-    <t>julia@gamil.com</t>
-  </si>
-  <si>
     <t>debora@gmail.com</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Adm</t>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>erik@gmail.com</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>Cassiana</t>
+  </si>
+  <si>
+    <t>cassiana@gmail.com</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>helena@gmail.com</t>
+  </si>
+  <si>
+    <t>roberto@gmail.com</t>
+  </si>
+  <si>
+    <t>Roberto</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +412,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,17 +513,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -519,12 +522,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,20 +539,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -557,6 +570,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
+      <color rgb="FF006699"/>
       <color rgb="FFC0C0C0"/>
       <color rgb="FF969696"/>
       <color rgb="FFFF9900"/>
@@ -565,8 +580,6 @@
       <color rgb="FFCC99FF"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FF0099CC"/>
-      <color rgb="FF003366"/>
-      <color rgb="FFCC0066"/>
     </mruColors>
   </colors>
   <extLst>
@@ -879,17 +892,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3359C9-2BD4-4328-B2D6-36C1F8EE747B}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
@@ -912,771 +925,877 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>43690</v>
       </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
         <v>4</v>
       </c>
-      <c r="I3" s="6">
-        <v>1</v>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="22">
+        <v>1</v>
+      </c>
+      <c r="K3" s="22">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>43256</v>
       </c>
-      <c r="F4" s="6">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="6">
-        <v>2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>2</v>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2</v>
+      </c>
+      <c r="J4" s="22">
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>42469</v>
       </c>
-      <c r="F5" s="6">
-        <v>2</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
         <v>6</v>
       </c>
-      <c r="H5" s="6">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6">
-        <v>2</v>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2</v>
+      </c>
+      <c r="J5" s="22">
+        <v>1</v>
+      </c>
+      <c r="K5" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
         <v>8</v>
       </c>
-      <c r="H6" s="6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="6">
-        <v>2</v>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" s="22">
+        <v>2</v>
+      </c>
+      <c r="K6" s="22">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>44505</v>
       </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <v>5</v>
       </c>
-      <c r="H7" s="6">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>3</v>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="22">
+        <v>3</v>
+      </c>
+      <c r="K7" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>43740</v>
       </c>
-      <c r="F8" s="6">
-        <v>2</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>3</v>
-      </c>
-      <c r="I8" s="6">
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
         <v>4</v>
       </c>
+      <c r="J8" s="22">
+        <v>3</v>
+      </c>
+      <c r="K8" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>43449</v>
       </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>2</v>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2</v>
+      </c>
+      <c r="J9" s="22">
+        <v>7</v>
+      </c>
+      <c r="K9" s="22">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>2</v>
-      </c>
-      <c r="H10" s="6">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>3</v>
+      <c r="E10" s="4">
+        <v>44671</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="22">
+        <v>11</v>
+      </c>
+      <c r="K10" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="E11" s="4">
+        <v>32549</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3">
         <v>7</v>
       </c>
-      <c r="H11" s="6">
-        <v>3</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="H11" s="3">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3">
         <v>4</v>
       </c>
+      <c r="J11" s="22">
+        <v>11</v>
+      </c>
+      <c r="K11" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6">
+      <c r="E12" s="4">
+        <v>40743</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
         <v>8</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="3">
         <v>4</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <v>5</v>
       </c>
+      <c r="J12" s="22">
+        <v>11</v>
+      </c>
+      <c r="K12" s="22">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="E13" s="4">
+        <v>43587</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="6">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1</v>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="22">
+        <v>11</v>
+      </c>
+      <c r="K13" s="22">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6">
-        <v>3</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="E14" s="4">
+        <v>42794</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3">
         <v>8</v>
       </c>
-      <c r="H14" s="6">
-        <v>2</v>
-      </c>
-      <c r="I14" s="6">
-        <v>2</v>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
+      </c>
+      <c r="J14" s="22">
+        <v>11</v>
+      </c>
+      <c r="K14" s="22">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
+      <c r="E15" s="4">
+        <v>43579</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
         <v>4</v>
       </c>
-      <c r="H15" s="6">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="22">
+        <v>12</v>
+      </c>
+      <c r="K15" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="E16" s="4">
+        <v>43940</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
         <v>5</v>
       </c>
-      <c r="H16" s="6">
-        <v>3</v>
-      </c>
-      <c r="I16" s="6">
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
         <v>5</v>
       </c>
+      <c r="J16" s="22">
+        <v>14</v>
+      </c>
+      <c r="K16" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="E17" s="4">
+        <v>40454</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3">
         <v>6</v>
       </c>
-      <c r="H17" s="6">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="3">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3">
         <v>4</v>
       </c>
+      <c r="J17" s="22">
+        <v>14</v>
+      </c>
+      <c r="K17" s="22">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="17" t="s">
+      <c r="H18" s="18"/>
+      <c r="I18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="9" t="s">
+      <c r="J18" s="20"/>
+      <c r="K18" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L18" s="9"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E20" s="8">
+        <v>37735</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E21" s="8">
+        <v>37735</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="9">
+        <v>2</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="6">
+        <v>2</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E22" s="8">
+        <v>37735</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="9">
+        <v>3</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="6">
+        <v>3</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3110</v>
+      </c>
+      <c r="E23" s="8">
+        <v>37735</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="6">
+        <v>4</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="5">
-        <v>123456</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="C24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3110</v>
+      </c>
+      <c r="E24" s="8">
         <v>37735</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="16">
-        <v>1</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="10">
-        <v>1</v>
-      </c>
-      <c r="L20" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="5">
-        <v>654321</v>
-      </c>
-      <c r="E21" s="12">
-        <v>37735</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="4">
-        <v>2</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="16">
-        <v>2</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="10">
-        <v>2</v>
-      </c>
-      <c r="L21" s="10" t="s">
+      <c r="F24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="6">
+        <v>5</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <v>7</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="10">
+        <v>2</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="5">
-        <v>112233</v>
-      </c>
-      <c r="E22" s="12">
-        <v>37735</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="4">
-        <v>3</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="16">
-        <v>3</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="10">
-        <v>3</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="10">
+        <v>3</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="10">
         <v>4</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="5">
-        <v>445566</v>
-      </c>
-      <c r="E23" s="12">
-        <v>37735</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="4">
-        <v>4</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="10">
-        <v>4</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>5</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="5">
-        <v>111111</v>
-      </c>
-      <c r="E24" s="12">
-        <v>37735</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="4">
-        <v>5</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="10">
-        <v>5</v>
-      </c>
-      <c r="L24" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="4">
-        <v>6</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="21">
-        <v>1</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G26" s="4">
-        <v>7</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="21">
-        <v>2</v>
-      </c>
-      <c r="J26" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G27" s="4">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I27" s="21">
-        <v>3</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I28" s="21">
-        <v>4</v>
-      </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="10" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>